<commit_message>
#93 게임서버 session -> character
</commit_message>
<xml_diff>
--- a/resources/table/enum.xlsx
+++ b/resources/table/enum.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\CSHYEON\Data\git\game\c++\fb\resources\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC9A117-EFF0-403D-86B3-C0E2CEC0BCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF825DCA-B7CE-49FA-9C09-3B266F89476A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{08B6B988-6A34-4205-94C2-FA55368096A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{08B6B988-6A34-4205-94C2-FA55368096A2}"/>
   </bookViews>
   <sheets>
     <sheet name="SEX" sheetId="1" r:id="rId1"/>
@@ -92,10 +92,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SESSION</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>LIFE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -104,10 +100,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MOB | SESSION</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ITEM | NPC | MOB</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -435,6 +427,14 @@
   </si>
   <si>
     <t>DEAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHARACTER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MOB | CHARACTER</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -895,50 +895,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -963,58 +963,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1040,58 +1040,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1117,98 +1117,98 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1232,66 +1232,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1312,18 +1312,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1344,34 +1344,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1392,34 +1392,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1440,18 +1440,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1515,15 +1515,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6499859-0EA3-4C78-B4A3-FBC5B2C22947}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -1531,7 +1531,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1547,8 +1547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489DB575-F218-4B7C-A32A-5F4BB8C4273D}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -1563,7 +1563,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1571,7 +1571,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1579,7 +1579,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1587,31 +1587,31 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1635,34 +1635,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1686,18 +1686,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1721,58 +1721,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1796,58 +1796,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1871,50 +1871,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>